<commit_message>
changes and physiology notes
</commit_message>
<xml_diff>
--- a/Mouse_workbooks/CH_090414_A.xlsx
+++ b/Mouse_workbooks/CH_090414_A.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\docubase\Mouse_workbooks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="140" windowWidth="25600" windowHeight="16060" tabRatio="738"/>
+    <workbookView xWindow="1185" yWindow="135" windowWidth="25605" windowHeight="16065" tabRatio="738"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="Surgery" sheetId="4" r:id="rId4"/>
     <sheet name="Analysis" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t>Mouse ID</t>
   </si>
@@ -151,7 +156,127 @@
     <t>No ear tags</t>
   </si>
   <si>
-    <t>Injected AAV2/1.ChR2 into V1.</t>
+    <t>2014_09_19_0001</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>2014_09_19_0002</t>
+  </si>
+  <si>
+    <t>2014_09_19_0003</t>
+  </si>
+  <si>
+    <t>OptoIV from a SOM cell (HS1) and a PY cell (HS2). Pulse width is 1 ms. 10 volts to LED, which targets (27 -59). The inhibition onto the PY cell is pretty weak. Vhold = +15 mV.</t>
+  </si>
+  <si>
+    <t>OptoIV from a SOM cell (HS1) and a PY cell (HS2). Pulse width is 1 ms. 10 volts to LED, which targets (27 -59). The inhibition onto the PY cell is pretty weak. Repeat of _0001.  Vhold = +15 mV.</t>
+  </si>
+  <si>
+    <t>OptoIV from a SOM cell (HS1) and a PY cell (HS2). Pulse width is 1 ms. 10 volts to LED, which targets (27 -59).  Vhold = +15 mV. FS open. Vhold = -75 mV.</t>
+  </si>
+  <si>
+    <t>OptoIV from a SOM cell (HS1) and a PY cell (HS2). Pulse width is 1 ms. 10 volts to LED, which targets (27 -59).  Vhold = +15 mV. FS open. Vhold = -75 mV. Pretty crummy access now (and before too.)</t>
+  </si>
+  <si>
+    <t>2014_09_19_0004</t>
+  </si>
+  <si>
+    <t>picture on crash. Not much data collected. I think that expression is weak and that I can't drive E/I that well. Moving on…</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>2014_09_19_0005</t>
+  </si>
+  <si>
+    <t>OptoIV from a SOM cell (HS1) and an unknown cell (HS2, possibly PY). HS2 receives lots of spontaneous inhibition at +15. Here, the LED was set to 6 volts and targets (-26 -7) FS open, 250 usec. Vhold = +15 for HS1, +17 for HS2.</t>
+  </si>
+  <si>
+    <t>2014_09_19_0006</t>
+  </si>
+  <si>
+    <t>OptoIV at -72 mV. LED set to 6 volts. HS1 receives more spontaneous excitation than HS2, consistent with HS1 being the SOM+ cell. FF excitation onto SOM+ cell is weaker than PY cell.</t>
+  </si>
+  <si>
+    <t>2014_09_19_0007</t>
+  </si>
+  <si>
+    <t>2014_09_19_0008</t>
+  </si>
+  <si>
+    <t>2014_09_19_0009</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OptoIV at -72 mV. LED set to 6 volts. HS1 receives more spontaneous excitation than HS2, consistent with HS1 being the SOM+ cell. FF excitation onto SOM+ cell is weaker than PY cell. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Now the LED targets (153 -109) FS open.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OptoIV at -72 mV. LED set to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>10 volts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">. HS1 receives more spontaneous excitation than HS2, consistent with HS1 being the SOM+ cell. FF excitation onto SOM+ cell is weaker than PY cell. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Now the LED targets (153 -109) FS closed.</t>
+    </r>
+  </si>
+  <si>
+    <t>OptoIV. Vhold = +15 for HS1, +19 for HS2. Multiple runs with 3 different volatages to the LED. Trying to see if E/I ratio depends on LED volatage. LED targets (-11 -16) FS open. Files _0009 to _0014</t>
+  </si>
+  <si>
+    <t>2014_09_19_0015</t>
+  </si>
+  <si>
+    <t>OptoIV. Vhold = +15 for HS1, +19 for HS2. Multiple runs with 3 different volatages to the LED. Trying to see if E/I ratio depends on LED volatage. LED targets (-11 -16) FS open. Files _0015 to _0022</t>
+  </si>
+  <si>
+    <t>Cell on HS1 at (-83 39), Vout = mV. Cell on HS2 at (6 25), Vout = mV. Pia at (-484 246)</t>
+  </si>
+  <si>
+    <t>Cs-Gluconate</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Trying to record E/I ratios from SOM+ and PY cells. Limited success. Also looked at stability of E/I ratio with different LED pulse intensities and distance.</t>
+  </si>
+  <si>
+    <t>Injected AAV2/1.ChR2 into V1. Whole cell recording. Histology.</t>
   </si>
 </sst>
 </file>
@@ -690,7 +815,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -801,6 +926,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -809,15 +946,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -908,6 +1036,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -919,21 +1062,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1288,14 +1416,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="38" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="38.1" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="62.33203125" style="27" customWidth="1"/>
+    <col min="1" max="1" width="20.625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="62.375" style="27" customWidth="1"/>
     <col min="3" max="16384" width="18.5" style="9" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="38" customHeight="1" thickTop="1">
+    <row r="1" spans="1:2" ht="38.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1303,7 +1431,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="38" customHeight="1">
+    <row r="2" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
@@ -1311,7 +1439,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="38" customHeight="1">
+    <row r="3" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
@@ -1319,7 +1447,7 @@
         <v>41856</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="38" customHeight="1">
+    <row r="4" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
@@ -1327,7 +1455,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="38" customHeight="1">
+    <row r="5" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
@@ -1335,27 +1463,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="148" customHeight="1" thickBot="1">
+    <row r="6" spans="1:2" ht="147.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="38" hidden="1" customHeight="1" thickTop="1"/>
-    <row r="8" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="9" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="10" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="11" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="12" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="13" spans="1:2" ht="38" hidden="1" customHeight="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="38.1" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>
@@ -1369,91 +1497,103 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:I7"/>
+      <selection activeCell="C4" sqref="C4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" style="35" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.125" style="35" customWidth="1"/>
+    <col min="6" max="6" width="7.125" style="21" customWidth="1"/>
     <col min="7" max="7" width="34.5" style="21" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.625" style="1" customWidth="1"/>
     <col min="10" max="16384" width="15" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39" customHeight="1" thickTop="1">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:9" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
       <c r="H1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="22"/>
-    </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1">
-      <c r="A2" s="53" t="s">
+      <c r="I1" s="22">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
       <c r="H2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="24"/>
-    </row>
-    <row r="3" spans="1:9" ht="39" customHeight="1">
-      <c r="A3" s="53" t="s">
+      <c r="I2" s="24">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="46"/>
-    </row>
-    <row r="4" spans="1:9" ht="102" customHeight="1" thickBot="1">
-      <c r="A4" s="55" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="45">
+        <v>34</v>
+      </c>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="47"/>
+    </row>
+    <row r="4" spans="1:9" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="50"/>
-    </row>
-    <row r="5" spans="1:9" ht="26" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-    </row>
-    <row r="6" spans="1:9" ht="39" customHeight="1" thickTop="1">
+      <c r="B4" s="57"/>
+      <c r="C4" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+    </row>
+    <row r="5" spans="1:9" ht="26.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+    </row>
+    <row r="6" spans="1:9" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -1472,1049 +1612,1295 @@
       <c r="F6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="41"/>
-      <c r="I6" s="42"/>
-    </row>
-    <row r="7" spans="1:9" ht="39" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="39"/>
-    </row>
-    <row r="8" spans="1:9" ht="39" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="39"/>
-    </row>
-    <row r="9" spans="1:9" ht="39" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="39"/>
-    </row>
-    <row r="10" spans="1:9" ht="39" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="39"/>
-    </row>
-    <row r="11" spans="1:9" ht="39" customHeight="1">
-      <c r="A11" s="3"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="40"/>
+    </row>
+    <row r="7" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="5">
+        <v>6</v>
+      </c>
+      <c r="E7" s="36">
+        <v>34</v>
+      </c>
+      <c r="F7" s="23">
+        <v>15</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="42"/>
+      <c r="I7" s="43"/>
+    </row>
+    <row r="8" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="37">
+        <v>6</v>
+      </c>
+      <c r="E8" s="36">
+        <v>34</v>
+      </c>
+      <c r="F8" s="23">
+        <v>15</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="42"/>
+      <c r="I8" s="43"/>
+    </row>
+    <row r="9" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="37">
+        <v>6</v>
+      </c>
+      <c r="E9" s="36">
+        <v>34</v>
+      </c>
+      <c r="F9" s="23">
+        <v>-75</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="42"/>
+      <c r="I9" s="43"/>
+    </row>
+    <row r="10" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="37">
+        <v>6</v>
+      </c>
+      <c r="E10" s="37">
+        <v>34</v>
+      </c>
+      <c r="F10" s="23">
+        <v>-72</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="42"/>
+      <c r="I10" s="43"/>
+    </row>
+    <row r="11" spans="1:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
+      <c r="D11" s="37">
+        <v>6</v>
+      </c>
       <c r="E11" s="36"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="39"/>
-    </row>
-    <row r="12" spans="1:9" ht="39" customHeight="1">
+      <c r="F11" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="42"/>
+      <c r="I11" s="43"/>
+    </row>
+    <row r="12" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="36"/>
       <c r="F12" s="23"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="39"/>
-    </row>
-    <row r="13" spans="1:9" ht="39" customHeight="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="39"/>
-    </row>
-    <row r="14" spans="1:9" ht="39" customHeight="1">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
-    </row>
-    <row r="15" spans="1:9" ht="39" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="39"/>
-    </row>
-    <row r="16" spans="1:9" ht="39" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="39"/>
-    </row>
-    <row r="17" spans="1:9" ht="39" customHeight="1">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="39"/>
-    </row>
-    <row r="18" spans="1:9" ht="39" customHeight="1">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="39"/>
-    </row>
-    <row r="19" spans="1:9" ht="39" customHeight="1">
-      <c r="A19" s="3"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="43"/>
+    </row>
+    <row r="13" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>2</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="5">
+        <v>5</v>
+      </c>
+      <c r="E13" s="36">
+        <v>34</v>
+      </c>
+      <c r="F13" s="23">
+        <v>15</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="42"/>
+      <c r="I13" s="43"/>
+    </row>
+    <row r="14" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5</v>
+      </c>
+      <c r="E14" s="36">
+        <v>34</v>
+      </c>
+      <c r="F14" s="23">
+        <v>-72</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="42"/>
+      <c r="I14" s="43"/>
+    </row>
+    <row r="15" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="37">
+        <v>5</v>
+      </c>
+      <c r="E15" s="37">
+        <v>34</v>
+      </c>
+      <c r="F15" s="37">
+        <v>-72</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="42"/>
+      <c r="I15" s="43"/>
+    </row>
+    <row r="16" spans="1:9" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="37">
+        <v>5</v>
+      </c>
+      <c r="E16" s="37">
+        <v>34</v>
+      </c>
+      <c r="F16" s="37">
+        <v>-72</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="42"/>
+      <c r="I16" s="43"/>
+    </row>
+    <row r="17" spans="1:9" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="37">
+        <v>5</v>
+      </c>
+      <c r="E17" s="37">
+        <v>34</v>
+      </c>
+      <c r="F17" s="23">
+        <v>15</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="42"/>
+      <c r="I17" s="43"/>
+    </row>
+    <row r="18" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>2</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="37">
+        <v>5</v>
+      </c>
+      <c r="E18" s="37">
+        <v>34</v>
+      </c>
+      <c r="F18" s="23">
+        <v>-72</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="42"/>
+      <c r="I18" s="43"/>
+    </row>
+    <row r="19" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>2</v>
+      </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
+      <c r="D19" s="5">
+        <v>5</v>
+      </c>
       <c r="E19" s="36"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="39"/>
-    </row>
-    <row r="20" spans="1:9" ht="39" customHeight="1">
+      <c r="F19" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" s="42"/>
+      <c r="I19" s="43"/>
+    </row>
+    <row r="20" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
       <c r="E20" s="36"/>
       <c r="F20" s="23"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-    </row>
-    <row r="21" spans="1:9" ht="39" customHeight="1">
+      <c r="G20" s="41"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="43"/>
+    </row>
+    <row r="21" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
       <c r="E21" s="36"/>
       <c r="F21" s="23"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="39"/>
-    </row>
-    <row r="22" spans="1:9" ht="39" customHeight="1">
+      <c r="G21" s="41"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="43"/>
+    </row>
+    <row r="22" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
       <c r="E22" s="36"/>
       <c r="F22" s="23"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="39"/>
-    </row>
-    <row r="23" spans="1:9" ht="39" customHeight="1">
+      <c r="G22" s="41"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="43"/>
+    </row>
+    <row r="23" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="5"/>
       <c r="E23" s="36"/>
       <c r="F23" s="23"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="39"/>
-    </row>
-    <row r="24" spans="1:9" ht="39" customHeight="1">
+      <c r="G23" s="41"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="43"/>
+    </row>
+    <row r="24" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="5"/>
       <c r="E24" s="36"/>
       <c r="F24" s="23"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="39"/>
-    </row>
-    <row r="25" spans="1:9" ht="39" customHeight="1">
+      <c r="G24" s="41"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="43"/>
+    </row>
+    <row r="25" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="5"/>
       <c r="E25" s="36"/>
       <c r="F25" s="23"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="39"/>
-    </row>
-    <row r="26" spans="1:9" ht="39" customHeight="1">
+      <c r="G25" s="41"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="43"/>
+    </row>
+    <row r="26" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="5"/>
       <c r="E26" s="36"/>
       <c r="F26" s="23"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="39"/>
-    </row>
-    <row r="27" spans="1:9" ht="39" customHeight="1">
+      <c r="G26" s="41"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="43"/>
+    </row>
+    <row r="27" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="5"/>
       <c r="E27" s="36"/>
       <c r="F27" s="23"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="39"/>
-    </row>
-    <row r="28" spans="1:9" ht="39" customHeight="1">
+      <c r="G27" s="41"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="43"/>
+    </row>
+    <row r="28" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="5"/>
       <c r="E28" s="36"/>
       <c r="F28" s="23"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="39"/>
-    </row>
-    <row r="29" spans="1:9" ht="39" customHeight="1">
+      <c r="G28" s="41"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="43"/>
+    </row>
+    <row r="29" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="5"/>
       <c r="E29" s="36"/>
       <c r="F29" s="23"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="39"/>
-    </row>
-    <row r="30" spans="1:9" ht="39" customHeight="1">
+      <c r="G29" s="41"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="43"/>
+    </row>
+    <row r="30" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="5"/>
       <c r="E30" s="36"/>
       <c r="F30" s="23"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="39"/>
-    </row>
-    <row r="31" spans="1:9" ht="39" customHeight="1">
+      <c r="G30" s="41"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="43"/>
+    </row>
+    <row r="31" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="5"/>
       <c r="E31" s="36"/>
       <c r="F31" s="23"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="39"/>
-    </row>
-    <row r="32" spans="1:9" ht="39" customHeight="1">
+      <c r="G31" s="41"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="43"/>
+    </row>
+    <row r="32" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="5"/>
       <c r="E32" s="36"/>
       <c r="F32" s="23"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="39"/>
-    </row>
-    <row r="33" spans="1:9" ht="39" customHeight="1">
+      <c r="G32" s="41"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="43"/>
+    </row>
+    <row r="33" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="5"/>
       <c r="E33" s="36"/>
       <c r="F33" s="23"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="39"/>
-    </row>
-    <row r="34" spans="1:9" ht="39" customHeight="1">
+      <c r="G33" s="41"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="43"/>
+    </row>
+    <row r="34" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="5"/>
       <c r="E34" s="36"/>
       <c r="F34" s="23"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="39"/>
-    </row>
-    <row r="35" spans="1:9" ht="39" customHeight="1">
+      <c r="G34" s="41"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="43"/>
+    </row>
+    <row r="35" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="5"/>
       <c r="E35" s="36"/>
       <c r="F35" s="23"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="39"/>
-    </row>
-    <row r="36" spans="1:9" ht="39" customHeight="1">
+      <c r="G35" s="41"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="43"/>
+    </row>
+    <row r="36" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="5"/>
       <c r="E36" s="36"/>
       <c r="F36" s="23"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="38"/>
-      <c r="I36" s="39"/>
-    </row>
-    <row r="37" spans="1:9" ht="39" customHeight="1">
+      <c r="G36" s="41"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="43"/>
+    </row>
+    <row r="37" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="5"/>
       <c r="E37" s="36"/>
       <c r="F37" s="23"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="39"/>
-    </row>
-    <row r="38" spans="1:9" ht="39" customHeight="1">
+      <c r="G37" s="41"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="43"/>
+    </row>
+    <row r="38" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="5"/>
       <c r="E38" s="36"/>
       <c r="F38" s="23"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="39"/>
-    </row>
-    <row r="39" spans="1:9" ht="39" customHeight="1">
+      <c r="G38" s="41"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="43"/>
+    </row>
+    <row r="39" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="5"/>
       <c r="E39" s="36"/>
       <c r="F39" s="23"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="38"/>
-      <c r="I39" s="39"/>
-    </row>
-    <row r="40" spans="1:9" ht="39" customHeight="1">
+      <c r="G39" s="41"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="43"/>
+    </row>
+    <row r="40" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="5"/>
       <c r="E40" s="36"/>
       <c r="F40" s="23"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="39"/>
-    </row>
-    <row r="41" spans="1:9" ht="39" customHeight="1">
+      <c r="G40" s="41"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="43"/>
+    </row>
+    <row r="41" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="5"/>
       <c r="E41" s="36"/>
       <c r="F41" s="23"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="39"/>
-    </row>
-    <row r="42" spans="1:9" ht="39" customHeight="1">
+      <c r="G41" s="41"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="43"/>
+    </row>
+    <row r="42" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="5"/>
       <c r="E42" s="36"/>
       <c r="F42" s="23"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="39"/>
-    </row>
-    <row r="43" spans="1:9" ht="39" customHeight="1">
+      <c r="G42" s="41"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="43"/>
+    </row>
+    <row r="43" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="5"/>
       <c r="E43" s="36"/>
       <c r="F43" s="23"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="39"/>
-    </row>
-    <row r="44" spans="1:9" ht="39" customHeight="1">
+      <c r="G43" s="41"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="43"/>
+    </row>
+    <row r="44" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="5"/>
       <c r="E44" s="36"/>
       <c r="F44" s="23"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="39"/>
-    </row>
-    <row r="45" spans="1:9" ht="39" customHeight="1">
+      <c r="G44" s="41"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="43"/>
+    </row>
+    <row r="45" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="5"/>
       <c r="E45" s="36"/>
       <c r="F45" s="23"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="39"/>
-    </row>
-    <row r="46" spans="1:9" ht="39" customHeight="1">
+      <c r="G45" s="41"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="43"/>
+    </row>
+    <row r="46" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="5"/>
       <c r="E46" s="36"/>
       <c r="F46" s="23"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="39"/>
-    </row>
-    <row r="47" spans="1:9" ht="39" customHeight="1">
+      <c r="G46" s="41"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="43"/>
+    </row>
+    <row r="47" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
       <c r="E47" s="36"/>
       <c r="F47" s="23"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-    </row>
-    <row r="48" spans="1:9" ht="39" customHeight="1">
+      <c r="G47" s="41"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="43"/>
+    </row>
+    <row r="48" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="5"/>
       <c r="E48" s="36"/>
       <c r="F48" s="23"/>
-      <c r="G48" s="37"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="39"/>
-    </row>
-    <row r="49" spans="1:9" ht="39" customHeight="1">
+      <c r="G48" s="41"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="43"/>
+    </row>
+    <row r="49" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="5"/>
       <c r="E49" s="36"/>
       <c r="F49" s="23"/>
-      <c r="G49" s="37"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="39"/>
-    </row>
-    <row r="50" spans="1:9" ht="39" customHeight="1">
+      <c r="G49" s="41"/>
+      <c r="H49" s="42"/>
+      <c r="I49" s="43"/>
+    </row>
+    <row r="50" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="5"/>
       <c r="E50" s="36"/>
       <c r="F50" s="23"/>
-      <c r="G50" s="37"/>
-      <c r="H50" s="38"/>
-      <c r="I50" s="39"/>
-    </row>
-    <row r="51" spans="1:9" ht="39" customHeight="1">
+      <c r="G50" s="41"/>
+      <c r="H50" s="42"/>
+      <c r="I50" s="43"/>
+    </row>
+    <row r="51" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="5"/>
       <c r="E51" s="36"/>
       <c r="F51" s="23"/>
-      <c r="G51" s="37"/>
-      <c r="H51" s="38"/>
-      <c r="I51" s="39"/>
-    </row>
-    <row r="52" spans="1:9" ht="39" customHeight="1">
+      <c r="G51" s="41"/>
+      <c r="H51" s="42"/>
+      <c r="I51" s="43"/>
+    </row>
+    <row r="52" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="5"/>
       <c r="E52" s="36"/>
       <c r="F52" s="23"/>
-      <c r="G52" s="37"/>
-      <c r="H52" s="38"/>
-      <c r="I52" s="39"/>
-    </row>
-    <row r="53" spans="1:9" ht="39" customHeight="1">
+      <c r="G52" s="41"/>
+      <c r="H52" s="42"/>
+      <c r="I52" s="43"/>
+    </row>
+    <row r="53" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="5"/>
       <c r="E53" s="36"/>
       <c r="F53" s="23"/>
-      <c r="G53" s="37"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="39"/>
-    </row>
-    <row r="54" spans="1:9" ht="39" customHeight="1">
+      <c r="G53" s="41"/>
+      <c r="H53" s="42"/>
+      <c r="I53" s="43"/>
+    </row>
+    <row r="54" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
       <c r="E54" s="36"/>
       <c r="F54" s="23"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="39"/>
-    </row>
-    <row r="55" spans="1:9" ht="39" customHeight="1">
+      <c r="G54" s="41"/>
+      <c r="H54" s="42"/>
+      <c r="I54" s="43"/>
+    </row>
+    <row r="55" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
       <c r="E55" s="36"/>
       <c r="F55" s="23"/>
-      <c r="G55" s="37"/>
-      <c r="H55" s="38"/>
-      <c r="I55" s="39"/>
-    </row>
-    <row r="56" spans="1:9" ht="39" customHeight="1">
+      <c r="G55" s="41"/>
+      <c r="H55" s="42"/>
+      <c r="I55" s="43"/>
+    </row>
+    <row r="56" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
       <c r="E56" s="36"/>
       <c r="F56" s="23"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="38"/>
-      <c r="I56" s="39"/>
-    </row>
-    <row r="57" spans="1:9" ht="39" customHeight="1">
+      <c r="G56" s="41"/>
+      <c r="H56" s="42"/>
+      <c r="I56" s="43"/>
+    </row>
+    <row r="57" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
       <c r="E57" s="36"/>
       <c r="F57" s="23"/>
-      <c r="G57" s="37"/>
-      <c r="H57" s="38"/>
-      <c r="I57" s="39"/>
-    </row>
-    <row r="58" spans="1:9" ht="39" customHeight="1">
+      <c r="G57" s="41"/>
+      <c r="H57" s="42"/>
+      <c r="I57" s="43"/>
+    </row>
+    <row r="58" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
       <c r="E58" s="36"/>
       <c r="F58" s="23"/>
-      <c r="G58" s="37"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="39"/>
-    </row>
-    <row r="59" spans="1:9" ht="39" customHeight="1">
+      <c r="G58" s="41"/>
+      <c r="H58" s="42"/>
+      <c r="I58" s="43"/>
+    </row>
+    <row r="59" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
       <c r="E59" s="36"/>
       <c r="F59" s="23"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="38"/>
-      <c r="I59" s="39"/>
-    </row>
-    <row r="60" spans="1:9" ht="39" customHeight="1">
+      <c r="G59" s="41"/>
+      <c r="H59" s="42"/>
+      <c r="I59" s="43"/>
+    </row>
+    <row r="60" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
       <c r="E60" s="36"/>
       <c r="F60" s="23"/>
-      <c r="G60" s="37"/>
-      <c r="H60" s="38"/>
-      <c r="I60" s="39"/>
-    </row>
-    <row r="61" spans="1:9" ht="39" customHeight="1">
+      <c r="G60" s="41"/>
+      <c r="H60" s="42"/>
+      <c r="I60" s="43"/>
+    </row>
+    <row r="61" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
       <c r="E61" s="36"/>
       <c r="F61" s="23"/>
-      <c r="G61" s="37"/>
-      <c r="H61" s="38"/>
-      <c r="I61" s="39"/>
-    </row>
-    <row r="62" spans="1:9" ht="39" customHeight="1">
+      <c r="G61" s="41"/>
+      <c r="H61" s="42"/>
+      <c r="I61" s="43"/>
+    </row>
+    <row r="62" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="5"/>
       <c r="E62" s="36"/>
       <c r="F62" s="23"/>
-      <c r="G62" s="37"/>
-      <c r="H62" s="38"/>
-      <c r="I62" s="39"/>
-    </row>
-    <row r="63" spans="1:9" ht="39" customHeight="1">
+      <c r="G62" s="41"/>
+      <c r="H62" s="42"/>
+      <c r="I62" s="43"/>
+    </row>
+    <row r="63" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="5"/>
       <c r="E63" s="36"/>
       <c r="F63" s="23"/>
-      <c r="G63" s="37"/>
-      <c r="H63" s="38"/>
-      <c r="I63" s="39"/>
-    </row>
-    <row r="64" spans="1:9" ht="39" customHeight="1">
+      <c r="G63" s="41"/>
+      <c r="H63" s="42"/>
+      <c r="I63" s="43"/>
+    </row>
+    <row r="64" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="5"/>
       <c r="E64" s="36"/>
       <c r="F64" s="23"/>
-      <c r="G64" s="37"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="39"/>
-    </row>
-    <row r="65" spans="1:9" ht="39" customHeight="1">
+      <c r="G64" s="41"/>
+      <c r="H64" s="42"/>
+      <c r="I64" s="43"/>
+    </row>
+    <row r="65" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="5"/>
       <c r="E65" s="36"/>
       <c r="F65" s="23"/>
-      <c r="G65" s="37"/>
-      <c r="H65" s="38"/>
-      <c r="I65" s="39"/>
-    </row>
-    <row r="66" spans="1:9" ht="39" customHeight="1">
+      <c r="G65" s="41"/>
+      <c r="H65" s="42"/>
+      <c r="I65" s="43"/>
+    </row>
+    <row r="66" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="5"/>
       <c r="E66" s="36"/>
       <c r="F66" s="23"/>
-      <c r="G66" s="37"/>
-      <c r="H66" s="38"/>
-      <c r="I66" s="39"/>
-    </row>
-    <row r="67" spans="1:9" ht="39" customHeight="1">
+      <c r="G66" s="41"/>
+      <c r="H66" s="42"/>
+      <c r="I66" s="43"/>
+    </row>
+    <row r="67" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="5"/>
       <c r="E67" s="36"/>
       <c r="F67" s="23"/>
-      <c r="G67" s="37"/>
-      <c r="H67" s="38"/>
-      <c r="I67" s="39"/>
-    </row>
-    <row r="68" spans="1:9" ht="39" customHeight="1">
+      <c r="G67" s="41"/>
+      <c r="H67" s="42"/>
+      <c r="I67" s="43"/>
+    </row>
+    <row r="68" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="5"/>
       <c r="E68" s="36"/>
       <c r="F68" s="23"/>
-      <c r="G68" s="37"/>
-      <c r="H68" s="38"/>
-      <c r="I68" s="39"/>
-    </row>
-    <row r="69" spans="1:9" ht="39" customHeight="1">
+      <c r="G68" s="41"/>
+      <c r="H68" s="42"/>
+      <c r="I68" s="43"/>
+    </row>
+    <row r="69" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="5"/>
       <c r="E69" s="36"/>
       <c r="F69" s="23"/>
-      <c r="G69" s="37"/>
-      <c r="H69" s="38"/>
-      <c r="I69" s="39"/>
-    </row>
-    <row r="70" spans="1:9" ht="39" customHeight="1">
+      <c r="G69" s="41"/>
+      <c r="H69" s="42"/>
+      <c r="I69" s="43"/>
+    </row>
+    <row r="70" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="5"/>
       <c r="E70" s="36"/>
       <c r="F70" s="23"/>
-      <c r="G70" s="37"/>
-      <c r="H70" s="38"/>
-      <c r="I70" s="39"/>
-    </row>
-    <row r="71" spans="1:9" ht="39" customHeight="1">
+      <c r="G70" s="41"/>
+      <c r="H70" s="42"/>
+      <c r="I70" s="43"/>
+    </row>
+    <row r="71" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="5"/>
       <c r="E71" s="36"/>
       <c r="F71" s="23"/>
-      <c r="G71" s="37"/>
-      <c r="H71" s="38"/>
-      <c r="I71" s="39"/>
-    </row>
-    <row r="72" spans="1:9" ht="39" customHeight="1">
+      <c r="G71" s="41"/>
+      <c r="H71" s="42"/>
+      <c r="I71" s="43"/>
+    </row>
+    <row r="72" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="5"/>
       <c r="E72" s="36"/>
       <c r="F72" s="23"/>
-      <c r="G72" s="37"/>
-      <c r="H72" s="38"/>
-      <c r="I72" s="39"/>
-    </row>
-    <row r="73" spans="1:9" ht="39" customHeight="1">
+      <c r="G72" s="41"/>
+      <c r="H72" s="42"/>
+      <c r="I72" s="43"/>
+    </row>
+    <row r="73" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
       <c r="E73" s="36"/>
       <c r="F73" s="23"/>
-      <c r="G73" s="37"/>
-      <c r="H73" s="38"/>
-      <c r="I73" s="39"/>
-    </row>
-    <row r="74" spans="1:9" ht="39" customHeight="1">
+      <c r="G73" s="41"/>
+      <c r="H73" s="42"/>
+      <c r="I73" s="43"/>
+    </row>
+    <row r="74" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="5"/>
       <c r="E74" s="36"/>
       <c r="F74" s="23"/>
-      <c r="G74" s="37"/>
-      <c r="H74" s="38"/>
-      <c r="I74" s="39"/>
-    </row>
-    <row r="75" spans="1:9" ht="39" customHeight="1">
+      <c r="G74" s="41"/>
+      <c r="H74" s="42"/>
+      <c r="I74" s="43"/>
+    </row>
+    <row r="75" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="5"/>
       <c r="E75" s="36"/>
       <c r="F75" s="23"/>
-      <c r="G75" s="37"/>
-      <c r="H75" s="38"/>
-      <c r="I75" s="39"/>
-    </row>
-    <row r="76" spans="1:9" ht="39" customHeight="1">
+      <c r="G75" s="41"/>
+      <c r="H75" s="42"/>
+      <c r="I75" s="43"/>
+    </row>
+    <row r="76" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="5"/>
       <c r="E76" s="36"/>
       <c r="F76" s="23"/>
-      <c r="G76" s="37"/>
-      <c r="H76" s="38"/>
-      <c r="I76" s="39"/>
-    </row>
-    <row r="77" spans="1:9" ht="39" customHeight="1">
+      <c r="G76" s="41"/>
+      <c r="H76" s="42"/>
+      <c r="I76" s="43"/>
+    </row>
+    <row r="77" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="5"/>
       <c r="E77" s="36"/>
       <c r="F77" s="23"/>
-      <c r="G77" s="37"/>
-      <c r="H77" s="38"/>
-      <c r="I77" s="39"/>
-    </row>
-    <row r="78" spans="1:9" ht="39" customHeight="1">
+      <c r="G77" s="41"/>
+      <c r="H77" s="42"/>
+      <c r="I77" s="43"/>
+    </row>
+    <row r="78" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="5"/>
       <c r="E78" s="36"/>
       <c r="F78" s="23"/>
-      <c r="G78" s="37"/>
-      <c r="H78" s="38"/>
-      <c r="I78" s="39"/>
-    </row>
-    <row r="79" spans="1:9" ht="39" customHeight="1">
+      <c r="G78" s="41"/>
+      <c r="H78" s="42"/>
+      <c r="I78" s="43"/>
+    </row>
+    <row r="79" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="5"/>
       <c r="E79" s="36"/>
       <c r="F79" s="23"/>
-      <c r="G79" s="37"/>
-      <c r="H79" s="38"/>
-      <c r="I79" s="39"/>
-    </row>
-    <row r="80" spans="1:9" ht="39" customHeight="1">
+      <c r="G79" s="41"/>
+      <c r="H79" s="42"/>
+      <c r="I79" s="43"/>
+    </row>
+    <row r="80" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="5"/>
       <c r="E80" s="36"/>
       <c r="F80" s="23"/>
-      <c r="G80" s="37"/>
-      <c r="H80" s="38"/>
-      <c r="I80" s="39"/>
-    </row>
-    <row r="81" spans="1:9" ht="39" customHeight="1">
+      <c r="G80" s="41"/>
+      <c r="H80" s="42"/>
+      <c r="I80" s="43"/>
+    </row>
+    <row r="81" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="5"/>
       <c r="E81" s="36"/>
       <c r="F81" s="23"/>
-      <c r="G81" s="37"/>
-      <c r="H81" s="38"/>
-      <c r="I81" s="39"/>
-    </row>
-    <row r="82" spans="1:9" ht="39" customHeight="1">
+      <c r="G81" s="41"/>
+      <c r="H81" s="42"/>
+      <c r="I81" s="43"/>
+    </row>
+    <row r="82" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="5"/>
       <c r="E82" s="36"/>
       <c r="F82" s="23"/>
-      <c r="G82" s="37"/>
-      <c r="H82" s="38"/>
-      <c r="I82" s="39"/>
-    </row>
-    <row r="83" spans="1:9" ht="39" customHeight="1">
+      <c r="G82" s="41"/>
+      <c r="H82" s="42"/>
+      <c r="I82" s="43"/>
+    </row>
+    <row r="83" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="5"/>
       <c r="E83" s="36"/>
       <c r="F83" s="23"/>
-      <c r="G83" s="37"/>
-      <c r="H83" s="38"/>
-      <c r="I83" s="39"/>
-    </row>
-    <row r="84" spans="1:9" ht="39" customHeight="1">
+      <c r="G83" s="41"/>
+      <c r="H83" s="42"/>
+      <c r="I83" s="43"/>
+    </row>
+    <row r="84" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="5"/>
       <c r="E84" s="36"/>
       <c r="F84" s="23"/>
-      <c r="G84" s="37"/>
-      <c r="H84" s="38"/>
-      <c r="I84" s="39"/>
-    </row>
-    <row r="85" spans="1:9" ht="39" customHeight="1">
+      <c r="G84" s="41"/>
+      <c r="H84" s="42"/>
+      <c r="I84" s="43"/>
+    </row>
+    <row r="85" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="5"/>
       <c r="E85" s="36"/>
       <c r="F85" s="23"/>
-      <c r="G85" s="37"/>
-      <c r="H85" s="38"/>
-      <c r="I85" s="39"/>
-    </row>
-    <row r="86" spans="1:9" ht="39" customHeight="1">
+      <c r="G85" s="41"/>
+      <c r="H85" s="42"/>
+      <c r="I85" s="43"/>
+    </row>
+    <row r="86" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="5"/>
       <c r="E86" s="36"/>
       <c r="F86" s="23"/>
-      <c r="G86" s="37"/>
-      <c r="H86" s="38"/>
-      <c r="I86" s="39"/>
-    </row>
-    <row r="87" spans="1:9" ht="39" customHeight="1">
+      <c r="G86" s="41"/>
+      <c r="H86" s="42"/>
+      <c r="I86" s="43"/>
+    </row>
+    <row r="87" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="5"/>
       <c r="E87" s="36"/>
       <c r="F87" s="23"/>
-      <c r="G87" s="37"/>
-      <c r="H87" s="38"/>
-      <c r="I87" s="39"/>
-    </row>
-    <row r="88" spans="1:9" ht="39" customHeight="1">
+      <c r="G87" s="41"/>
+      <c r="H87" s="42"/>
+      <c r="I87" s="43"/>
+    </row>
+    <row r="88" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="5"/>
       <c r="E88" s="36"/>
       <c r="F88" s="23"/>
-      <c r="G88" s="37"/>
-      <c r="H88" s="38"/>
-      <c r="I88" s="39"/>
-    </row>
-    <row r="89" spans="1:9" ht="39" customHeight="1">
+      <c r="G88" s="41"/>
+      <c r="H88" s="42"/>
+      <c r="I88" s="43"/>
+    </row>
+    <row r="89" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="5"/>
       <c r="E89" s="36"/>
       <c r="F89" s="23"/>
-      <c r="G89" s="37"/>
-      <c r="H89" s="38"/>
-      <c r="I89" s="39"/>
-    </row>
-    <row r="90" spans="1:9" ht="39" customHeight="1">
+      <c r="G89" s="41"/>
+      <c r="H89" s="42"/>
+      <c r="I89" s="43"/>
+    </row>
+    <row r="90" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="5"/>
       <c r="E90" s="36"/>
       <c r="F90" s="23"/>
-      <c r="G90" s="37"/>
-      <c r="H90" s="38"/>
-      <c r="I90" s="39"/>
-    </row>
-    <row r="91" spans="1:9" ht="39" customHeight="1">
+      <c r="G90" s="41"/>
+      <c r="H90" s="42"/>
+      <c r="I90" s="43"/>
+    </row>
+    <row r="91" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="5"/>
       <c r="E91" s="36"/>
       <c r="F91" s="23"/>
-      <c r="G91" s="37"/>
-      <c r="H91" s="38"/>
-      <c r="I91" s="39"/>
-    </row>
-    <row r="92" spans="1:9" ht="39" customHeight="1">
+      <c r="G91" s="41"/>
+      <c r="H91" s="42"/>
+      <c r="I91" s="43"/>
+    </row>
+    <row r="92" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="5"/>
       <c r="E92" s="36"/>
       <c r="F92" s="23"/>
-      <c r="G92" s="37"/>
-      <c r="H92" s="38"/>
-      <c r="I92" s="39"/>
-    </row>
-    <row r="93" spans="1:9" ht="39" customHeight="1">
+      <c r="G92" s="41"/>
+      <c r="H92" s="42"/>
+      <c r="I92" s="43"/>
+    </row>
+    <row r="93" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="5"/>
       <c r="E93" s="36"/>
       <c r="F93" s="23"/>
-      <c r="G93" s="37"/>
-      <c r="H93" s="38"/>
-      <c r="I93" s="39"/>
-    </row>
-    <row r="94" spans="1:9" ht="39" customHeight="1">
+      <c r="G93" s="41"/>
+      <c r="H93" s="42"/>
+      <c r="I93" s="43"/>
+    </row>
+    <row r="94" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="5"/>
       <c r="E94" s="36"/>
       <c r="F94" s="23"/>
-      <c r="G94" s="37"/>
-      <c r="H94" s="38"/>
-      <c r="I94" s="39"/>
-    </row>
-    <row r="95" spans="1:9" ht="39" customHeight="1">
+      <c r="G94" s="41"/>
+      <c r="H94" s="42"/>
+      <c r="I94" s="43"/>
+    </row>
+    <row r="95" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="5"/>
       <c r="E95" s="36"/>
       <c r="F95" s="23"/>
-      <c r="G95" s="37"/>
-      <c r="H95" s="38"/>
-      <c r="I95" s="39"/>
-    </row>
-    <row r="96" spans="1:9" ht="39" customHeight="1">
+      <c r="G95" s="41"/>
+      <c r="H95" s="42"/>
+      <c r="I95" s="43"/>
+    </row>
+    <row r="96" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="5"/>
       <c r="E96" s="36"/>
       <c r="F96" s="23"/>
-      <c r="G96" s="37"/>
-      <c r="H96" s="38"/>
-      <c r="I96" s="39"/>
-    </row>
-    <row r="97" spans="1:9" ht="39" customHeight="1">
+      <c r="G96" s="41"/>
+      <c r="H96" s="42"/>
+      <c r="I96" s="43"/>
+    </row>
+    <row r="97" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="5"/>
       <c r="E97" s="36"/>
       <c r="F97" s="23"/>
-      <c r="G97" s="37"/>
-      <c r="H97" s="38"/>
-      <c r="I97" s="39"/>
-    </row>
-    <row r="98" spans="1:9" ht="39" customHeight="1">
+      <c r="G97" s="41"/>
+      <c r="H97" s="42"/>
+      <c r="I97" s="43"/>
+    </row>
+    <row r="98" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="5"/>
       <c r="E98" s="36"/>
       <c r="F98" s="23"/>
-      <c r="G98" s="37"/>
-      <c r="H98" s="38"/>
-      <c r="I98" s="39"/>
-    </row>
-    <row r="99" spans="1:9" ht="39" customHeight="1">
+      <c r="G98" s="41"/>
+      <c r="H98" s="42"/>
+      <c r="I98" s="43"/>
+    </row>
+    <row r="99" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="5"/>
       <c r="E99" s="36"/>
       <c r="F99" s="23"/>
-      <c r="G99" s="37"/>
-      <c r="H99" s="38"/>
-      <c r="I99" s="39"/>
-    </row>
-    <row r="100" spans="1:9" ht="39" customHeight="1">
+      <c r="G99" s="41"/>
+      <c r="H99" s="42"/>
+      <c r="I99" s="43"/>
+    </row>
+    <row r="100" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="5"/>
       <c r="E100" s="36"/>
       <c r="F100" s="23"/>
-      <c r="G100" s="37"/>
-      <c r="H100" s="38"/>
-      <c r="I100" s="39"/>
-    </row>
-    <row r="101" spans="1:9" ht="39" hidden="1" customHeight="1" thickTop="1"/>
+      <c r="G100" s="41"/>
+      <c r="H100" s="42"/>
+      <c r="I100" s="43"/>
+    </row>
+    <row r="101" spans="1:9" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="104">
+    <mergeCell ref="G96:I96"/>
+    <mergeCell ref="G97:I97"/>
+    <mergeCell ref="G98:I98"/>
+    <mergeCell ref="G99:I99"/>
+    <mergeCell ref="G100:I100"/>
+    <mergeCell ref="G91:I91"/>
+    <mergeCell ref="G92:I92"/>
+    <mergeCell ref="G93:I93"/>
+    <mergeCell ref="G94:I94"/>
+    <mergeCell ref="G95:I95"/>
+    <mergeCell ref="G86:I86"/>
+    <mergeCell ref="G87:I87"/>
+    <mergeCell ref="G88:I88"/>
+    <mergeCell ref="G89:I89"/>
+    <mergeCell ref="G90:I90"/>
+    <mergeCell ref="G81:I81"/>
+    <mergeCell ref="G82:I82"/>
+    <mergeCell ref="G83:I83"/>
+    <mergeCell ref="G84:I84"/>
+    <mergeCell ref="G85:I85"/>
+    <mergeCell ref="G76:I76"/>
+    <mergeCell ref="G77:I77"/>
+    <mergeCell ref="G78:I78"/>
+    <mergeCell ref="G79:I79"/>
+    <mergeCell ref="G80:I80"/>
+    <mergeCell ref="G71:I71"/>
+    <mergeCell ref="G72:I72"/>
+    <mergeCell ref="G73:I73"/>
+    <mergeCell ref="G74:I74"/>
+    <mergeCell ref="G75:I75"/>
+    <mergeCell ref="G66:I66"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="G69:I69"/>
+    <mergeCell ref="G70:I70"/>
+    <mergeCell ref="G61:I61"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="G63:I63"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="G56:I56"/>
+    <mergeCell ref="G57:I57"/>
+    <mergeCell ref="G58:I58"/>
+    <mergeCell ref="G59:I59"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="G54:I54"/>
+    <mergeCell ref="G55:I55"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G8:I8"/>
@@ -2529,100 +2915,10 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="C2:G2"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="G56:I56"/>
-    <mergeCell ref="G57:I57"/>
-    <mergeCell ref="G58:I58"/>
-    <mergeCell ref="G59:I59"/>
-    <mergeCell ref="G60:I60"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="G53:I53"/>
-    <mergeCell ref="G54:I54"/>
-    <mergeCell ref="G55:I55"/>
-    <mergeCell ref="G66:I66"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="G68:I68"/>
-    <mergeCell ref="G69:I69"/>
-    <mergeCell ref="G70:I70"/>
-    <mergeCell ref="G61:I61"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="G63:I63"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="G65:I65"/>
-    <mergeCell ref="G76:I76"/>
-    <mergeCell ref="G77:I77"/>
-    <mergeCell ref="G78:I78"/>
-    <mergeCell ref="G79:I79"/>
-    <mergeCell ref="G80:I80"/>
-    <mergeCell ref="G71:I71"/>
-    <mergeCell ref="G72:I72"/>
-    <mergeCell ref="G73:I73"/>
-    <mergeCell ref="G74:I74"/>
-    <mergeCell ref="G75:I75"/>
-    <mergeCell ref="G86:I86"/>
-    <mergeCell ref="G87:I87"/>
-    <mergeCell ref="G88:I88"/>
-    <mergeCell ref="G89:I89"/>
-    <mergeCell ref="G90:I90"/>
-    <mergeCell ref="G81:I81"/>
-    <mergeCell ref="G82:I82"/>
-    <mergeCell ref="G83:I83"/>
-    <mergeCell ref="G84:I84"/>
-    <mergeCell ref="G85:I85"/>
-    <mergeCell ref="G96:I96"/>
-    <mergeCell ref="G97:I97"/>
-    <mergeCell ref="G98:I98"/>
-    <mergeCell ref="G99:I99"/>
-    <mergeCell ref="G100:I100"/>
-    <mergeCell ref="G91:I91"/>
-    <mergeCell ref="G92:I92"/>
-    <mergeCell ref="G93:I93"/>
-    <mergeCell ref="G94:I94"/>
-    <mergeCell ref="G95:I95"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.47222222222222221" right="0.56944444444444442" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2635,95 +2931,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E4"/>
+    <sheetView view="pageLayout" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="21.875" style="17" customWidth="1"/>
     <col min="2" max="4" width="15" style="17" customWidth="1"/>
     <col min="5" max="5" width="16.5" style="17" customWidth="1"/>
     <col min="6" max="16384" width="15" style="17" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="36" customHeight="1">
+    <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="60"/>
-    </row>
-    <row r="2" spans="1:5" ht="36" customHeight="1">
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="61"/>
+    </row>
+    <row r="2" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="62"/>
-    </row>
-    <row r="3" spans="1:5" ht="136" customHeight="1">
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="63"/>
+    </row>
+    <row r="3" spans="1:5" ht="135.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="64"/>
-    </row>
-    <row r="4" spans="1:5" ht="46" customHeight="1">
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="65"/>
+    </row>
+    <row r="4" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="69"/>
-    </row>
-    <row r="5" spans="1:5" ht="46" customHeight="1">
+      <c r="B4" s="68">
+        <v>300</v>
+      </c>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="70"/>
+    </row>
+    <row r="5" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="64"/>
-    </row>
-    <row r="6" spans="1:5" ht="46" customHeight="1">
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="65"/>
+    </row>
+    <row r="6" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="64"/>
-    </row>
-    <row r="7" spans="1:5" ht="46" customHeight="1">
+      <c r="B6" s="64">
+        <v>2</v>
+      </c>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="65"/>
+    </row>
+    <row r="7" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="69"/>
-    </row>
-    <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1">
+      <c r="B7" s="68">
+        <v>6</v>
+      </c>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="70"/>
+    </row>
+    <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="66"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2738,7 +3040,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -2755,209 +3057,209 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="2" customWidth="1"/>
-    <col min="2" max="6" width="10.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2" hidden="1"/>
+    <col min="1" max="1" width="14.125" style="2" customWidth="1"/>
+    <col min="2" max="6" width="10.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="36" customHeight="1">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="72"/>
-    </row>
-    <row r="2" spans="1:7" ht="36" customHeight="1">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="73"/>
+    </row>
+    <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="81">
+      <c r="B2" s="74">
         <v>41886</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="64"/>
-    </row>
-    <row r="3" spans="1:7" ht="36" customHeight="1">
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="65"/>
+    </row>
+    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="64"/>
-    </row>
-    <row r="4" spans="1:7" ht="112" customHeight="1">
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="65"/>
+    </row>
+    <row r="4" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="64"/>
-    </row>
-    <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1">
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="65"/>
+    </row>
+    <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="66"/>
-    </row>
-    <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1"/>
-    <row r="7" spans="1:7" ht="36" customHeight="1">
-      <c r="A7" s="70" t="s">
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="67"/>
+    </row>
+    <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="72"/>
-    </row>
-    <row r="8" spans="1:7" ht="36" customHeight="1">
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="73"/>
+    </row>
+    <row r="8" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="78"/>
-    </row>
-    <row r="9" spans="1:7" ht="36" customHeight="1">
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="76"/>
+    </row>
+    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="64"/>
-    </row>
-    <row r="10" spans="1:7" ht="112" customHeight="1">
+      <c r="B9" s="64"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="65"/>
+    </row>
+    <row r="10" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="64"/>
-    </row>
-    <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1">
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
+    </row>
+    <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="80"/>
-    </row>
-    <row r="12" spans="1:7" ht="36" customHeight="1"/>
-    <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1"/>
-    <row r="14" spans="1:7" ht="36" customHeight="1">
-      <c r="A14" s="70" t="s">
+      <c r="B11" s="77"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="78"/>
+    </row>
+    <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="71"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="72"/>
-    </row>
-    <row r="15" spans="1:7" ht="36" customHeight="1">
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="73"/>
+    </row>
+    <row r="15" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="74"/>
-    </row>
-    <row r="16" spans="1:7" ht="36" customHeight="1">
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="80"/>
+    </row>
+    <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="64"/>
-    </row>
-    <row r="17" spans="1:7" ht="113" customHeight="1">
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="65"/>
+    </row>
+    <row r="17" spans="1:7" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="64"/>
-    </row>
-    <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1">
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="65"/>
+    </row>
+    <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="76"/>
-    </row>
-    <row r="19" spans="1:7" ht="36" customHeight="1"/>
-    <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="82"/>
+    </row>
+    <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2976,7 +3278,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
changes to mouse workbooks.
</commit_message>
<xml_diff>
--- a/Mouse_workbooks/CH_090414_A.xlsx
+++ b/Mouse_workbooks/CH_090414_A.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="135" windowWidth="25605" windowHeight="16065" tabRatio="738"/>
+    <workbookView xWindow="1185" yWindow="135" windowWidth="25605" windowHeight="16065" tabRatio="738" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -174,12 +174,6 @@
     <t>OptoIV from a SOM cell (HS1) and a PY cell (HS2). Pulse width is 1 ms. 10 volts to LED, which targets (27 -59). The inhibition onto the PY cell is pretty weak. Repeat of _0001.  Vhold = +15 mV.</t>
   </si>
   <si>
-    <t>OptoIV from a SOM cell (HS1) and a PY cell (HS2). Pulse width is 1 ms. 10 volts to LED, which targets (27 -59).  Vhold = +15 mV. FS open. Vhold = -75 mV.</t>
-  </si>
-  <si>
-    <t>OptoIV from a SOM cell (HS1) and a PY cell (HS2). Pulse width is 1 ms. 10 volts to LED, which targets (27 -59).  Vhold = +15 mV. FS open. Vhold = -75 mV. Pretty crummy access now (and before too.)</t>
-  </si>
-  <si>
     <t>2014_09_19_0004</t>
   </si>
   <si>
@@ -277,6 +271,12 @@
   </si>
   <si>
     <t>Injected AAV2/1.ChR2 into V1. Whole cell recording. Histology.</t>
+  </si>
+  <si>
+    <t>OptoIV from a SOM cell (HS1) and a PY cell (HS2). Pulse width is 1 ms. 10 volts to LED, which targets (27 -59).  Vhold = -75 mV. FS open.</t>
+  </si>
+  <si>
+    <t>OptoIV from a SOM cell (HS1) and a PY cell (HS2). Pulse width is 1 ms. 10 volts to LED, which targets (27 -59).  FS open. Vhold = -72 mV. Pretty crummy access now (and before too.)</t>
   </si>
 </sst>
 </file>
@@ -928,15 +928,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -946,6 +937,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1036,32 +1036,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1412,7 +1412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1468,7 +1468,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="38.1" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -1496,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:I4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="58" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D1" s="59"/>
       <c r="E1" s="59"/>
@@ -1538,13 +1538,13 @@
         <v>8</v>
       </c>
       <c r="B2" s="55"/>
-      <c r="C2" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
+      <c r="C2" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
       <c r="H2" s="26" t="s">
         <v>30</v>
       </c>
@@ -1560,10 +1560,10 @@
       <c r="C3" s="45">
         <v>34</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
       <c r="H3" s="46"/>
       <c r="I3" s="47"/>
     </row>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="B4" s="57"/>
       <c r="C4" s="48" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="49"/>
@@ -1612,11 +1612,11 @@
       <c r="F6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="40"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="43"/>
     </row>
     <row r="7" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -1637,11 +1637,11 @@
       <c r="F7" s="23">
         <v>15</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G7" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="42"/>
-      <c r="I7" s="43"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="40"/>
     </row>
     <row r="8" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -1662,11 +1662,11 @@
       <c r="F8" s="23">
         <v>15</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="42"/>
-      <c r="I8" s="43"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="40"/>
     </row>
     <row r="9" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -1687,18 +1687,18 @@
       <c r="F9" s="23">
         <v>-75</v>
       </c>
-      <c r="G9" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="42"/>
-      <c r="I9" s="43"/>
+      <c r="G9" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="39"/>
+      <c r="I9" s="40"/>
     </row>
     <row r="10" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>43</v>
@@ -1712,11 +1712,11 @@
       <c r="F10" s="23">
         <v>-72</v>
       </c>
-      <c r="G10" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="42"/>
-      <c r="I10" s="43"/>
+      <c r="G10" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="39"/>
+      <c r="I10" s="40"/>
     </row>
     <row r="11" spans="1:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -1729,13 +1729,13 @@
       </c>
       <c r="E11" s="36"/>
       <c r="F11" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="H11" s="42"/>
-      <c r="I11" s="43"/>
+        <v>50</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="39"/>
+      <c r="I11" s="40"/>
     </row>
     <row r="12" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -1744,16 +1744,16 @@
       <c r="D12" s="5"/>
       <c r="E12" s="36"/>
       <c r="F12" s="23"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="43"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="40"/>
     </row>
     <row r="13" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>43</v>
@@ -1767,18 +1767,18 @@
       <c r="F13" s="23">
         <v>15</v>
       </c>
-      <c r="G13" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="42"/>
-      <c r="I13" s="43"/>
+      <c r="G13" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="39"/>
+      <c r="I13" s="40"/>
     </row>
     <row r="14" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>2</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>43</v>
@@ -1792,18 +1792,18 @@
       <c r="F14" s="23">
         <v>-72</v>
       </c>
-      <c r="G14" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" s="42"/>
-      <c r="I14" s="43"/>
+      <c r="G14" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="39"/>
+      <c r="I14" s="40"/>
     </row>
     <row r="15" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>43</v>
@@ -1817,18 +1817,18 @@
       <c r="F15" s="37">
         <v>-72</v>
       </c>
-      <c r="G15" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="42"/>
-      <c r="I15" s="43"/>
+      <c r="G15" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="39"/>
+      <c r="I15" s="40"/>
     </row>
     <row r="16" spans="1:9" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>43</v>
@@ -1842,18 +1842,18 @@
       <c r="F16" s="37">
         <v>-72</v>
       </c>
-      <c r="G16" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="42"/>
-      <c r="I16" s="43"/>
+      <c r="G16" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="39"/>
+      <c r="I16" s="40"/>
     </row>
     <row r="17" spans="1:9" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>43</v>
@@ -1867,18 +1867,18 @@
       <c r="F17" s="23">
         <v>15</v>
       </c>
-      <c r="G17" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="H17" s="42"/>
-      <c r="I17" s="43"/>
+      <c r="G17" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="39"/>
+      <c r="I17" s="40"/>
     </row>
     <row r="18" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>2</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>43</v>
@@ -1892,11 +1892,11 @@
       <c r="F18" s="23">
         <v>-72</v>
       </c>
-      <c r="G18" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" s="42"/>
-      <c r="I18" s="43"/>
+      <c r="G18" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="39"/>
+      <c r="I18" s="40"/>
     </row>
     <row r="19" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -1909,13 +1909,13 @@
       </c>
       <c r="E19" s="36"/>
       <c r="F19" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="H19" s="42"/>
-      <c r="I19" s="43"/>
+        <v>50</v>
+      </c>
+      <c r="G19" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="39"/>
+      <c r="I19" s="40"/>
     </row>
     <row r="20" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
@@ -1924,9 +1924,9 @@
       <c r="D20" s="5"/>
       <c r="E20" s="36"/>
       <c r="F20" s="23"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="43"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="40"/>
     </row>
     <row r="21" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -1935,9 +1935,9 @@
       <c r="D21" s="5"/>
       <c r="E21" s="36"/>
       <c r="F21" s="23"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="43"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="40"/>
     </row>
     <row r="22" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -1946,9 +1946,9 @@
       <c r="D22" s="5"/>
       <c r="E22" s="36"/>
       <c r="F22" s="23"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="43"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="40"/>
     </row>
     <row r="23" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
@@ -1957,9 +1957,9 @@
       <c r="D23" s="5"/>
       <c r="E23" s="36"/>
       <c r="F23" s="23"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="43"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="40"/>
     </row>
     <row r="24" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
@@ -1968,9 +1968,9 @@
       <c r="D24" s="5"/>
       <c r="E24" s="36"/>
       <c r="F24" s="23"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="43"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="40"/>
     </row>
     <row r="25" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -1979,9 +1979,9 @@
       <c r="D25" s="5"/>
       <c r="E25" s="36"/>
       <c r="F25" s="23"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="43"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="40"/>
     </row>
     <row r="26" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -1990,9 +1990,9 @@
       <c r="D26" s="5"/>
       <c r="E26" s="36"/>
       <c r="F26" s="23"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="43"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="40"/>
     </row>
     <row r="27" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
@@ -2001,9 +2001,9 @@
       <c r="D27" s="5"/>
       <c r="E27" s="36"/>
       <c r="F27" s="23"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="43"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="40"/>
     </row>
     <row r="28" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -2012,9 +2012,9 @@
       <c r="D28" s="5"/>
       <c r="E28" s="36"/>
       <c r="F28" s="23"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="43"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="40"/>
     </row>
     <row r="29" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -2023,9 +2023,9 @@
       <c r="D29" s="5"/>
       <c r="E29" s="36"/>
       <c r="F29" s="23"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="43"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="40"/>
     </row>
     <row r="30" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
@@ -2034,9 +2034,9 @@
       <c r="D30" s="5"/>
       <c r="E30" s="36"/>
       <c r="F30" s="23"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="43"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="40"/>
     </row>
     <row r="31" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
@@ -2045,9 +2045,9 @@
       <c r="D31" s="5"/>
       <c r="E31" s="36"/>
       <c r="F31" s="23"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="43"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="40"/>
     </row>
     <row r="32" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
@@ -2056,9 +2056,9 @@
       <c r="D32" s="5"/>
       <c r="E32" s="36"/>
       <c r="F32" s="23"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="43"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="40"/>
     </row>
     <row r="33" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
@@ -2067,9 +2067,9 @@
       <c r="D33" s="5"/>
       <c r="E33" s="36"/>
       <c r="F33" s="23"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="43"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="40"/>
     </row>
     <row r="34" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
@@ -2078,9 +2078,9 @@
       <c r="D34" s="5"/>
       <c r="E34" s="36"/>
       <c r="F34" s="23"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="43"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="40"/>
     </row>
     <row r="35" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
@@ -2089,9 +2089,9 @@
       <c r="D35" s="5"/>
       <c r="E35" s="36"/>
       <c r="F35" s="23"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="43"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="40"/>
     </row>
     <row r="36" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
@@ -2100,9 +2100,9 @@
       <c r="D36" s="5"/>
       <c r="E36" s="36"/>
       <c r="F36" s="23"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="43"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="40"/>
     </row>
     <row r="37" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
@@ -2111,9 +2111,9 @@
       <c r="D37" s="5"/>
       <c r="E37" s="36"/>
       <c r="F37" s="23"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="43"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="40"/>
     </row>
     <row r="38" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
@@ -2122,9 +2122,9 @@
       <c r="D38" s="5"/>
       <c r="E38" s="36"/>
       <c r="F38" s="23"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="43"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="40"/>
     </row>
     <row r="39" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
@@ -2133,9 +2133,9 @@
       <c r="D39" s="5"/>
       <c r="E39" s="36"/>
       <c r="F39" s="23"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="43"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="40"/>
     </row>
     <row r="40" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
@@ -2144,9 +2144,9 @@
       <c r="D40" s="5"/>
       <c r="E40" s="36"/>
       <c r="F40" s="23"/>
-      <c r="G40" s="41"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="43"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="40"/>
     </row>
     <row r="41" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
@@ -2155,9 +2155,9 @@
       <c r="D41" s="5"/>
       <c r="E41" s="36"/>
       <c r="F41" s="23"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="43"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="40"/>
     </row>
     <row r="42" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
@@ -2166,9 +2166,9 @@
       <c r="D42" s="5"/>
       <c r="E42" s="36"/>
       <c r="F42" s="23"/>
-      <c r="G42" s="41"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="43"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="40"/>
     </row>
     <row r="43" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
@@ -2177,9 +2177,9 @@
       <c r="D43" s="5"/>
       <c r="E43" s="36"/>
       <c r="F43" s="23"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="43"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="40"/>
     </row>
     <row r="44" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
@@ -2188,9 +2188,9 @@
       <c r="D44" s="5"/>
       <c r="E44" s="36"/>
       <c r="F44" s="23"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="43"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="40"/>
     </row>
     <row r="45" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
@@ -2199,9 +2199,9 @@
       <c r="D45" s="5"/>
       <c r="E45" s="36"/>
       <c r="F45" s="23"/>
-      <c r="G45" s="41"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="43"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="40"/>
     </row>
     <row r="46" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
@@ -2210,9 +2210,9 @@
       <c r="D46" s="5"/>
       <c r="E46" s="36"/>
       <c r="F46" s="23"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="43"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="39"/>
+      <c r="I46" s="40"/>
     </row>
     <row r="47" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
@@ -2221,9 +2221,9 @@
       <c r="D47" s="5"/>
       <c r="E47" s="36"/>
       <c r="F47" s="23"/>
-      <c r="G47" s="41"/>
-      <c r="H47" s="42"/>
-      <c r="I47" s="43"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="39"/>
+      <c r="I47" s="40"/>
     </row>
     <row r="48" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
@@ -2232,9 +2232,9 @@
       <c r="D48" s="5"/>
       <c r="E48" s="36"/>
       <c r="F48" s="23"/>
-      <c r="G48" s="41"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="43"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="39"/>
+      <c r="I48" s="40"/>
     </row>
     <row r="49" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
@@ -2243,9 +2243,9 @@
       <c r="D49" s="5"/>
       <c r="E49" s="36"/>
       <c r="F49" s="23"/>
-      <c r="G49" s="41"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="43"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="39"/>
+      <c r="I49" s="40"/>
     </row>
     <row r="50" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
@@ -2254,9 +2254,9 @@
       <c r="D50" s="5"/>
       <c r="E50" s="36"/>
       <c r="F50" s="23"/>
-      <c r="G50" s="41"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="43"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="39"/>
+      <c r="I50" s="40"/>
     </row>
     <row r="51" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
@@ -2265,9 +2265,9 @@
       <c r="D51" s="5"/>
       <c r="E51" s="36"/>
       <c r="F51" s="23"/>
-      <c r="G51" s="41"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="43"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="39"/>
+      <c r="I51" s="40"/>
     </row>
     <row r="52" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
@@ -2276,9 +2276,9 @@
       <c r="D52" s="5"/>
       <c r="E52" s="36"/>
       <c r="F52" s="23"/>
-      <c r="G52" s="41"/>
-      <c r="H52" s="42"/>
-      <c r="I52" s="43"/>
+      <c r="G52" s="38"/>
+      <c r="H52" s="39"/>
+      <c r="I52" s="40"/>
     </row>
     <row r="53" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
@@ -2287,9 +2287,9 @@
       <c r="D53" s="5"/>
       <c r="E53" s="36"/>
       <c r="F53" s="23"/>
-      <c r="G53" s="41"/>
-      <c r="H53" s="42"/>
-      <c r="I53" s="43"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="39"/>
+      <c r="I53" s="40"/>
     </row>
     <row r="54" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
@@ -2298,9 +2298,9 @@
       <c r="D54" s="5"/>
       <c r="E54" s="36"/>
       <c r="F54" s="23"/>
-      <c r="G54" s="41"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="43"/>
+      <c r="G54" s="38"/>
+      <c r="H54" s="39"/>
+      <c r="I54" s="40"/>
     </row>
     <row r="55" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
@@ -2309,9 +2309,9 @@
       <c r="D55" s="5"/>
       <c r="E55" s="36"/>
       <c r="F55" s="23"/>
-      <c r="G55" s="41"/>
-      <c r="H55" s="42"/>
-      <c r="I55" s="43"/>
+      <c r="G55" s="38"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="40"/>
     </row>
     <row r="56" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
@@ -2320,9 +2320,9 @@
       <c r="D56" s="5"/>
       <c r="E56" s="36"/>
       <c r="F56" s="23"/>
-      <c r="G56" s="41"/>
-      <c r="H56" s="42"/>
-      <c r="I56" s="43"/>
+      <c r="G56" s="38"/>
+      <c r="H56" s="39"/>
+      <c r="I56" s="40"/>
     </row>
     <row r="57" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
@@ -2331,9 +2331,9 @@
       <c r="D57" s="5"/>
       <c r="E57" s="36"/>
       <c r="F57" s="23"/>
-      <c r="G57" s="41"/>
-      <c r="H57" s="42"/>
-      <c r="I57" s="43"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="39"/>
+      <c r="I57" s="40"/>
     </row>
     <row r="58" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
@@ -2342,9 +2342,9 @@
       <c r="D58" s="5"/>
       <c r="E58" s="36"/>
       <c r="F58" s="23"/>
-      <c r="G58" s="41"/>
-      <c r="H58" s="42"/>
-      <c r="I58" s="43"/>
+      <c r="G58" s="38"/>
+      <c r="H58" s="39"/>
+      <c r="I58" s="40"/>
     </row>
     <row r="59" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
@@ -2353,9 +2353,9 @@
       <c r="D59" s="5"/>
       <c r="E59" s="36"/>
       <c r="F59" s="23"/>
-      <c r="G59" s="41"/>
-      <c r="H59" s="42"/>
-      <c r="I59" s="43"/>
+      <c r="G59" s="38"/>
+      <c r="H59" s="39"/>
+      <c r="I59" s="40"/>
     </row>
     <row r="60" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
@@ -2364,9 +2364,9 @@
       <c r="D60" s="5"/>
       <c r="E60" s="36"/>
       <c r="F60" s="23"/>
-      <c r="G60" s="41"/>
-      <c r="H60" s="42"/>
-      <c r="I60" s="43"/>
+      <c r="G60" s="38"/>
+      <c r="H60" s="39"/>
+      <c r="I60" s="40"/>
     </row>
     <row r="61" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
@@ -2375,9 +2375,9 @@
       <c r="D61" s="5"/>
       <c r="E61" s="36"/>
       <c r="F61" s="23"/>
-      <c r="G61" s="41"/>
-      <c r="H61" s="42"/>
-      <c r="I61" s="43"/>
+      <c r="G61" s="38"/>
+      <c r="H61" s="39"/>
+      <c r="I61" s="40"/>
     </row>
     <row r="62" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
@@ -2386,9 +2386,9 @@
       <c r="D62" s="5"/>
       <c r="E62" s="36"/>
       <c r="F62" s="23"/>
-      <c r="G62" s="41"/>
-      <c r="H62" s="42"/>
-      <c r="I62" s="43"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="39"/>
+      <c r="I62" s="40"/>
     </row>
     <row r="63" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
@@ -2397,9 +2397,9 @@
       <c r="D63" s="5"/>
       <c r="E63" s="36"/>
       <c r="F63" s="23"/>
-      <c r="G63" s="41"/>
-      <c r="H63" s="42"/>
-      <c r="I63" s="43"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="39"/>
+      <c r="I63" s="40"/>
     </row>
     <row r="64" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
@@ -2408,9 +2408,9 @@
       <c r="D64" s="5"/>
       <c r="E64" s="36"/>
       <c r="F64" s="23"/>
-      <c r="G64" s="41"/>
-      <c r="H64" s="42"/>
-      <c r="I64" s="43"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="39"/>
+      <c r="I64" s="40"/>
     </row>
     <row r="65" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
@@ -2419,9 +2419,9 @@
       <c r="D65" s="5"/>
       <c r="E65" s="36"/>
       <c r="F65" s="23"/>
-      <c r="G65" s="41"/>
-      <c r="H65" s="42"/>
-      <c r="I65" s="43"/>
+      <c r="G65" s="38"/>
+      <c r="H65" s="39"/>
+      <c r="I65" s="40"/>
     </row>
     <row r="66" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
@@ -2430,9 +2430,9 @@
       <c r="D66" s="5"/>
       <c r="E66" s="36"/>
       <c r="F66" s="23"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="42"/>
-      <c r="I66" s="43"/>
+      <c r="G66" s="38"/>
+      <c r="H66" s="39"/>
+      <c r="I66" s="40"/>
     </row>
     <row r="67" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
@@ -2441,9 +2441,9 @@
       <c r="D67" s="5"/>
       <c r="E67" s="36"/>
       <c r="F67" s="23"/>
-      <c r="G67" s="41"/>
-      <c r="H67" s="42"/>
-      <c r="I67" s="43"/>
+      <c r="G67" s="38"/>
+      <c r="H67" s="39"/>
+      <c r="I67" s="40"/>
     </row>
     <row r="68" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
@@ -2452,9 +2452,9 @@
       <c r="D68" s="5"/>
       <c r="E68" s="36"/>
       <c r="F68" s="23"/>
-      <c r="G68" s="41"/>
-      <c r="H68" s="42"/>
-      <c r="I68" s="43"/>
+      <c r="G68" s="38"/>
+      <c r="H68" s="39"/>
+      <c r="I68" s="40"/>
     </row>
     <row r="69" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
@@ -2463,9 +2463,9 @@
       <c r="D69" s="5"/>
       <c r="E69" s="36"/>
       <c r="F69" s="23"/>
-      <c r="G69" s="41"/>
-      <c r="H69" s="42"/>
-      <c r="I69" s="43"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="39"/>
+      <c r="I69" s="40"/>
     </row>
     <row r="70" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
@@ -2474,9 +2474,9 @@
       <c r="D70" s="5"/>
       <c r="E70" s="36"/>
       <c r="F70" s="23"/>
-      <c r="G70" s="41"/>
-      <c r="H70" s="42"/>
-      <c r="I70" s="43"/>
+      <c r="G70" s="38"/>
+      <c r="H70" s="39"/>
+      <c r="I70" s="40"/>
     </row>
     <row r="71" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
@@ -2485,9 +2485,9 @@
       <c r="D71" s="5"/>
       <c r="E71" s="36"/>
       <c r="F71" s="23"/>
-      <c r="G71" s="41"/>
-      <c r="H71" s="42"/>
-      <c r="I71" s="43"/>
+      <c r="G71" s="38"/>
+      <c r="H71" s="39"/>
+      <c r="I71" s="40"/>
     </row>
     <row r="72" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
@@ -2496,9 +2496,9 @@
       <c r="D72" s="5"/>
       <c r="E72" s="36"/>
       <c r="F72" s="23"/>
-      <c r="G72" s="41"/>
-      <c r="H72" s="42"/>
-      <c r="I72" s="43"/>
+      <c r="G72" s="38"/>
+      <c r="H72" s="39"/>
+      <c r="I72" s="40"/>
     </row>
     <row r="73" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
@@ -2507,9 +2507,9 @@
       <c r="D73" s="5"/>
       <c r="E73" s="36"/>
       <c r="F73" s="23"/>
-      <c r="G73" s="41"/>
-      <c r="H73" s="42"/>
-      <c r="I73" s="43"/>
+      <c r="G73" s="38"/>
+      <c r="H73" s="39"/>
+      <c r="I73" s="40"/>
     </row>
     <row r="74" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
@@ -2518,9 +2518,9 @@
       <c r="D74" s="5"/>
       <c r="E74" s="36"/>
       <c r="F74" s="23"/>
-      <c r="G74" s="41"/>
-      <c r="H74" s="42"/>
-      <c r="I74" s="43"/>
+      <c r="G74" s="38"/>
+      <c r="H74" s="39"/>
+      <c r="I74" s="40"/>
     </row>
     <row r="75" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
@@ -2529,9 +2529,9 @@
       <c r="D75" s="5"/>
       <c r="E75" s="36"/>
       <c r="F75" s="23"/>
-      <c r="G75" s="41"/>
-      <c r="H75" s="42"/>
-      <c r="I75" s="43"/>
+      <c r="G75" s="38"/>
+      <c r="H75" s="39"/>
+      <c r="I75" s="40"/>
     </row>
     <row r="76" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
@@ -2540,9 +2540,9 @@
       <c r="D76" s="5"/>
       <c r="E76" s="36"/>
       <c r="F76" s="23"/>
-      <c r="G76" s="41"/>
-      <c r="H76" s="42"/>
-      <c r="I76" s="43"/>
+      <c r="G76" s="38"/>
+      <c r="H76" s="39"/>
+      <c r="I76" s="40"/>
     </row>
     <row r="77" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
@@ -2551,9 +2551,9 @@
       <c r="D77" s="5"/>
       <c r="E77" s="36"/>
       <c r="F77" s="23"/>
-      <c r="G77" s="41"/>
-      <c r="H77" s="42"/>
-      <c r="I77" s="43"/>
+      <c r="G77" s="38"/>
+      <c r="H77" s="39"/>
+      <c r="I77" s="40"/>
     </row>
     <row r="78" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
@@ -2562,9 +2562,9 @@
       <c r="D78" s="5"/>
       <c r="E78" s="36"/>
       <c r="F78" s="23"/>
-      <c r="G78" s="41"/>
-      <c r="H78" s="42"/>
-      <c r="I78" s="43"/>
+      <c r="G78" s="38"/>
+      <c r="H78" s="39"/>
+      <c r="I78" s="40"/>
     </row>
     <row r="79" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
@@ -2573,9 +2573,9 @@
       <c r="D79" s="5"/>
       <c r="E79" s="36"/>
       <c r="F79" s="23"/>
-      <c r="G79" s="41"/>
-      <c r="H79" s="42"/>
-      <c r="I79" s="43"/>
+      <c r="G79" s="38"/>
+      <c r="H79" s="39"/>
+      <c r="I79" s="40"/>
     </row>
     <row r="80" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
@@ -2584,9 +2584,9 @@
       <c r="D80" s="5"/>
       <c r="E80" s="36"/>
       <c r="F80" s="23"/>
-      <c r="G80" s="41"/>
-      <c r="H80" s="42"/>
-      <c r="I80" s="43"/>
+      <c r="G80" s="38"/>
+      <c r="H80" s="39"/>
+      <c r="I80" s="40"/>
     </row>
     <row r="81" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
@@ -2595,9 +2595,9 @@
       <c r="D81" s="5"/>
       <c r="E81" s="36"/>
       <c r="F81" s="23"/>
-      <c r="G81" s="41"/>
-      <c r="H81" s="42"/>
-      <c r="I81" s="43"/>
+      <c r="G81" s="38"/>
+      <c r="H81" s="39"/>
+      <c r="I81" s="40"/>
     </row>
     <row r="82" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
@@ -2606,9 +2606,9 @@
       <c r="D82" s="5"/>
       <c r="E82" s="36"/>
       <c r="F82" s="23"/>
-      <c r="G82" s="41"/>
-      <c r="H82" s="42"/>
-      <c r="I82" s="43"/>
+      <c r="G82" s="38"/>
+      <c r="H82" s="39"/>
+      <c r="I82" s="40"/>
     </row>
     <row r="83" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
@@ -2617,9 +2617,9 @@
       <c r="D83" s="5"/>
       <c r="E83" s="36"/>
       <c r="F83" s="23"/>
-      <c r="G83" s="41"/>
-      <c r="H83" s="42"/>
-      <c r="I83" s="43"/>
+      <c r="G83" s="38"/>
+      <c r="H83" s="39"/>
+      <c r="I83" s="40"/>
     </row>
     <row r="84" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
@@ -2628,9 +2628,9 @@
       <c r="D84" s="5"/>
       <c r="E84" s="36"/>
       <c r="F84" s="23"/>
-      <c r="G84" s="41"/>
-      <c r="H84" s="42"/>
-      <c r="I84" s="43"/>
+      <c r="G84" s="38"/>
+      <c r="H84" s="39"/>
+      <c r="I84" s="40"/>
     </row>
     <row r="85" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
@@ -2639,9 +2639,9 @@
       <c r="D85" s="5"/>
       <c r="E85" s="36"/>
       <c r="F85" s="23"/>
-      <c r="G85" s="41"/>
-      <c r="H85" s="42"/>
-      <c r="I85" s="43"/>
+      <c r="G85" s="38"/>
+      <c r="H85" s="39"/>
+      <c r="I85" s="40"/>
     </row>
     <row r="86" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
@@ -2650,9 +2650,9 @@
       <c r="D86" s="5"/>
       <c r="E86" s="36"/>
       <c r="F86" s="23"/>
-      <c r="G86" s="41"/>
-      <c r="H86" s="42"/>
-      <c r="I86" s="43"/>
+      <c r="G86" s="38"/>
+      <c r="H86" s="39"/>
+      <c r="I86" s="40"/>
     </row>
     <row r="87" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
@@ -2661,9 +2661,9 @@
       <c r="D87" s="5"/>
       <c r="E87" s="36"/>
       <c r="F87" s="23"/>
-      <c r="G87" s="41"/>
-      <c r="H87" s="42"/>
-      <c r="I87" s="43"/>
+      <c r="G87" s="38"/>
+      <c r="H87" s="39"/>
+      <c r="I87" s="40"/>
     </row>
     <row r="88" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
@@ -2672,9 +2672,9 @@
       <c r="D88" s="5"/>
       <c r="E88" s="36"/>
       <c r="F88" s="23"/>
-      <c r="G88" s="41"/>
-      <c r="H88" s="42"/>
-      <c r="I88" s="43"/>
+      <c r="G88" s="38"/>
+      <c r="H88" s="39"/>
+      <c r="I88" s="40"/>
     </row>
     <row r="89" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
@@ -2683,9 +2683,9 @@
       <c r="D89" s="5"/>
       <c r="E89" s="36"/>
       <c r="F89" s="23"/>
-      <c r="G89" s="41"/>
-      <c r="H89" s="42"/>
-      <c r="I89" s="43"/>
+      <c r="G89" s="38"/>
+      <c r="H89" s="39"/>
+      <c r="I89" s="40"/>
     </row>
     <row r="90" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
@@ -2694,9 +2694,9 @@
       <c r="D90" s="5"/>
       <c r="E90" s="36"/>
       <c r="F90" s="23"/>
-      <c r="G90" s="41"/>
-      <c r="H90" s="42"/>
-      <c r="I90" s="43"/>
+      <c r="G90" s="38"/>
+      <c r="H90" s="39"/>
+      <c r="I90" s="40"/>
     </row>
     <row r="91" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
@@ -2705,9 +2705,9 @@
       <c r="D91" s="5"/>
       <c r="E91" s="36"/>
       <c r="F91" s="23"/>
-      <c r="G91" s="41"/>
-      <c r="H91" s="42"/>
-      <c r="I91" s="43"/>
+      <c r="G91" s="38"/>
+      <c r="H91" s="39"/>
+      <c r="I91" s="40"/>
     </row>
     <row r="92" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
@@ -2716,9 +2716,9 @@
       <c r="D92" s="5"/>
       <c r="E92" s="36"/>
       <c r="F92" s="23"/>
-      <c r="G92" s="41"/>
-      <c r="H92" s="42"/>
-      <c r="I92" s="43"/>
+      <c r="G92" s="38"/>
+      <c r="H92" s="39"/>
+      <c r="I92" s="40"/>
     </row>
     <row r="93" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
@@ -2727,9 +2727,9 @@
       <c r="D93" s="5"/>
       <c r="E93" s="36"/>
       <c r="F93" s="23"/>
-      <c r="G93" s="41"/>
-      <c r="H93" s="42"/>
-      <c r="I93" s="43"/>
+      <c r="G93" s="38"/>
+      <c r="H93" s="39"/>
+      <c r="I93" s="40"/>
     </row>
     <row r="94" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
@@ -2738,9 +2738,9 @@
       <c r="D94" s="5"/>
       <c r="E94" s="36"/>
       <c r="F94" s="23"/>
-      <c r="G94" s="41"/>
-      <c r="H94" s="42"/>
-      <c r="I94" s="43"/>
+      <c r="G94" s="38"/>
+      <c r="H94" s="39"/>
+      <c r="I94" s="40"/>
     </row>
     <row r="95" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
@@ -2749,9 +2749,9 @@
       <c r="D95" s="5"/>
       <c r="E95" s="36"/>
       <c r="F95" s="23"/>
-      <c r="G95" s="41"/>
-      <c r="H95" s="42"/>
-      <c r="I95" s="43"/>
+      <c r="G95" s="38"/>
+      <c r="H95" s="39"/>
+      <c r="I95" s="40"/>
     </row>
     <row r="96" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
@@ -2760,9 +2760,9 @@
       <c r="D96" s="5"/>
       <c r="E96" s="36"/>
       <c r="F96" s="23"/>
-      <c r="G96" s="41"/>
-      <c r="H96" s="42"/>
-      <c r="I96" s="43"/>
+      <c r="G96" s="38"/>
+      <c r="H96" s="39"/>
+      <c r="I96" s="40"/>
     </row>
     <row r="97" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
@@ -2771,9 +2771,9 @@
       <c r="D97" s="5"/>
       <c r="E97" s="36"/>
       <c r="F97" s="23"/>
-      <c r="G97" s="41"/>
-      <c r="H97" s="42"/>
-      <c r="I97" s="43"/>
+      <c r="G97" s="38"/>
+      <c r="H97" s="39"/>
+      <c r="I97" s="40"/>
     </row>
     <row r="98" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
@@ -2782,9 +2782,9 @@
       <c r="D98" s="5"/>
       <c r="E98" s="36"/>
       <c r="F98" s="23"/>
-      <c r="G98" s="41"/>
-      <c r="H98" s="42"/>
-      <c r="I98" s="43"/>
+      <c r="G98" s="38"/>
+      <c r="H98" s="39"/>
+      <c r="I98" s="40"/>
     </row>
     <row r="99" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
@@ -2793,9 +2793,9 @@
       <c r="D99" s="5"/>
       <c r="E99" s="36"/>
       <c r="F99" s="23"/>
-      <c r="G99" s="41"/>
-      <c r="H99" s="42"/>
-      <c r="I99" s="43"/>
+      <c r="G99" s="38"/>
+      <c r="H99" s="39"/>
+      <c r="I99" s="40"/>
     </row>
     <row r="100" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
@@ -2804,103 +2804,13 @@
       <c r="D100" s="5"/>
       <c r="E100" s="36"/>
       <c r="F100" s="23"/>
-      <c r="G100" s="41"/>
-      <c r="H100" s="42"/>
-      <c r="I100" s="43"/>
+      <c r="G100" s="38"/>
+      <c r="H100" s="39"/>
+      <c r="I100" s="40"/>
     </row>
     <row r="101" spans="1:9" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="G96:I96"/>
-    <mergeCell ref="G97:I97"/>
-    <mergeCell ref="G98:I98"/>
-    <mergeCell ref="G99:I99"/>
-    <mergeCell ref="G100:I100"/>
-    <mergeCell ref="G91:I91"/>
-    <mergeCell ref="G92:I92"/>
-    <mergeCell ref="G93:I93"/>
-    <mergeCell ref="G94:I94"/>
-    <mergeCell ref="G95:I95"/>
-    <mergeCell ref="G86:I86"/>
-    <mergeCell ref="G87:I87"/>
-    <mergeCell ref="G88:I88"/>
-    <mergeCell ref="G89:I89"/>
-    <mergeCell ref="G90:I90"/>
-    <mergeCell ref="G81:I81"/>
-    <mergeCell ref="G82:I82"/>
-    <mergeCell ref="G83:I83"/>
-    <mergeCell ref="G84:I84"/>
-    <mergeCell ref="G85:I85"/>
-    <mergeCell ref="G76:I76"/>
-    <mergeCell ref="G77:I77"/>
-    <mergeCell ref="G78:I78"/>
-    <mergeCell ref="G79:I79"/>
-    <mergeCell ref="G80:I80"/>
-    <mergeCell ref="G71:I71"/>
-    <mergeCell ref="G72:I72"/>
-    <mergeCell ref="G73:I73"/>
-    <mergeCell ref="G74:I74"/>
-    <mergeCell ref="G75:I75"/>
-    <mergeCell ref="G66:I66"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="G68:I68"/>
-    <mergeCell ref="G69:I69"/>
-    <mergeCell ref="G70:I70"/>
-    <mergeCell ref="G61:I61"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="G63:I63"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="G65:I65"/>
-    <mergeCell ref="G56:I56"/>
-    <mergeCell ref="G57:I57"/>
-    <mergeCell ref="G58:I58"/>
-    <mergeCell ref="G59:I59"/>
-    <mergeCell ref="G60:I60"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="G53:I53"/>
-    <mergeCell ref="G54:I54"/>
-    <mergeCell ref="G55:I55"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G8:I8"/>
@@ -2915,6 +2825,96 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="C2:G2"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="G56:I56"/>
+    <mergeCell ref="G57:I57"/>
+    <mergeCell ref="G58:I58"/>
+    <mergeCell ref="G59:I59"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="G54:I54"/>
+    <mergeCell ref="G55:I55"/>
+    <mergeCell ref="G66:I66"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="G69:I69"/>
+    <mergeCell ref="G70:I70"/>
+    <mergeCell ref="G61:I61"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="G63:I63"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="G76:I76"/>
+    <mergeCell ref="G77:I77"/>
+    <mergeCell ref="G78:I78"/>
+    <mergeCell ref="G79:I79"/>
+    <mergeCell ref="G80:I80"/>
+    <mergeCell ref="G71:I71"/>
+    <mergeCell ref="G72:I72"/>
+    <mergeCell ref="G73:I73"/>
+    <mergeCell ref="G74:I74"/>
+    <mergeCell ref="G75:I75"/>
+    <mergeCell ref="G86:I86"/>
+    <mergeCell ref="G87:I87"/>
+    <mergeCell ref="G88:I88"/>
+    <mergeCell ref="G89:I89"/>
+    <mergeCell ref="G90:I90"/>
+    <mergeCell ref="G81:I81"/>
+    <mergeCell ref="G82:I82"/>
+    <mergeCell ref="G83:I83"/>
+    <mergeCell ref="G84:I84"/>
+    <mergeCell ref="G85:I85"/>
+    <mergeCell ref="G96:I96"/>
+    <mergeCell ref="G97:I97"/>
+    <mergeCell ref="G98:I98"/>
+    <mergeCell ref="G99:I99"/>
+    <mergeCell ref="G100:I100"/>
+    <mergeCell ref="G91:I91"/>
+    <mergeCell ref="G92:I92"/>
+    <mergeCell ref="G93:I93"/>
+    <mergeCell ref="G94:I94"/>
+    <mergeCell ref="G95:I95"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.47222222222222221" right="0.56944444444444442" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3080,7 +3080,7 @@
       <c r="A2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="74">
+      <c r="B2" s="82">
         <v>41886</v>
       </c>
       <c r="C2" s="64"/>
@@ -3144,12 +3144,12 @@
       <c r="A8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="76"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="79"/>
     </row>
     <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
@@ -3177,12 +3177,12 @@
       <c r="A11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="78"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="81"/>
     </row>
     <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3201,12 +3201,12 @@
       <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="80"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="75"/>
     </row>
     <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
@@ -3234,32 +3234,32 @@
       <c r="A18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="81"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="81"/>
-      <c r="F18" s="81"/>
-      <c r="G18" s="82"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="77"/>
     </row>
     <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="B15:G15"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>